<commit_message>
todo sobre metadatos en HTML e inicio de mi portafolio
</commit_message>
<xml_diff>
--- a/Sena/Registro de Aprendisaje - Analisis y desarrollo de sistemas informaticos/Fase 1. identificación/Trabajos y sus directrises/7. Identificación del proceso de software para el proyecto de desarrollo en curso/Resuelto. Evidencia AP01-AA1-EV07 - Identificación del proceso de software para el proyecto de desarrollo en curso.xlsx
+++ b/Sena/Registro de Aprendisaje - Analisis y desarrollo de sistemas informaticos/Fase 1. identificación/Trabajos y sus directrises/7. Identificación del proceso de software para el proyecto de desarrollo en curso/Resuelto. Evidencia AP01-AA1-EV07 - Identificación del proceso de software para el proyecto de desarrollo en curso.xlsx
@@ -2058,7 +2058,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -2219,6 +2219,309 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -2369,7 +2672,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2518,19 +2821,178 @@
       <alignment horizontal="justify" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="20" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="21" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="22" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2852,8 +3314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C150"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C145" sqref="C145"/>
+    <sheetView topLeftCell="A101" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.000000"/>
@@ -2863,7 +3325,7 @@
     <col min="3" max="3" width="30.86214338" customWidth="1" outlineLevel="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" ht="16.500000">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="16.500000">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -2873,595 +3335,771 @@
       <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="45" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="106" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="88" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="89" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="39"/>
-      <c r="C7" s="39"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="B8" s="39"/>
-      <c r="C8" s="39"/>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="39"/>
-      <c r="C9" s="39"/>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" s="39"/>
-      <c r="C10" s="39"/>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-    </row>
-    <row r="12" spans="1:3">
-      <c r="B12" s="39"/>
-      <c r="C12" s="39"/>
-    </row>
-    <row r="13" spans="1:3">
-      <c r="B13" s="39"/>
-      <c r="C13" s="39"/>
-    </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="39"/>
-      <c r="C14" s="39"/>
-    </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="39"/>
-      <c r="C15" s="39"/>
-    </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="39"/>
-      <c r="C16" s="39"/>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="39"/>
-      <c r="C17" s="39"/>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="39"/>
-      <c r="C18" s="39"/>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="39"/>
-      <c r="C19" s="39"/>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="39"/>
-      <c r="C20" s="39"/>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="39"/>
-      <c r="C21" s="39"/>
-    </row>
-    <row r="22" spans="2:3">
-      <c r="B22" s="39"/>
-      <c r="C22" s="39"/>
-    </row>
-    <row r="23" spans="2:3">
-      <c r="B23" s="39"/>
-      <c r="C23" s="39"/>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="39"/>
-      <c r="C24" s="39"/>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="39"/>
-      <c r="C25" s="39"/>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="39"/>
-      <c r="C26" s="39"/>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="39"/>
-      <c r="C27" s="39"/>
-    </row>
-    <row r="28" spans="2:3">
-      <c r="B28" s="39"/>
-      <c r="C28" s="35"/>
-    </row>
-    <row r="29" spans="2:3">
-      <c r="B29" s="39"/>
-      <c r="C29" s="35"/>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="39"/>
-      <c r="C30" s="35"/>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="39"/>
-      <c r="C31" s="35"/>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="39"/>
-      <c r="C32" s="35"/>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="39"/>
-      <c r="C33" s="35"/>
-    </row>
-    <row r="34" spans="2:3">
-      <c r="B34" s="39"/>
-      <c r="C34" s="35"/>
-    </row>
-    <row r="35" spans="2:3">
-      <c r="B35" s="39"/>
-      <c r="C35" s="35"/>
-    </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="39"/>
-      <c r="C36" s="35"/>
-    </row>
-    <row r="37" spans="2:3">
-      <c r="B37" s="39"/>
-      <c r="C37" s="35"/>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="39"/>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="39"/>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="39"/>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="39"/>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="39"/>
-    </row>
-    <row r="43" spans="2:3">
-      <c r="B43" s="39"/>
-    </row>
-    <row r="44" spans="2:3">
-      <c r="B44" s="39"/>
-    </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="39"/>
-    </row>
-    <row r="46" spans="2:3">
-      <c r="B46" s="39"/>
-    </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="39"/>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="39"/>
+    <row r="3" spans="1:4">
+      <c r="A3" s="90"/>
+      <c r="B3" s="81"/>
+      <c r="C3" s="91"/>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="90"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="91"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="90"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="91"/>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="90"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="91"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="90"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="91"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="90"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="91"/>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="90"/>
+      <c r="B9" s="81"/>
+      <c r="C9" s="91"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="90"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="91"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="90"/>
+      <c r="B11" s="81"/>
+      <c r="C11" s="91"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="90"/>
+      <c r="B12" s="81"/>
+      <c r="C12" s="91"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="90"/>
+      <c r="B13" s="81"/>
+      <c r="C13" s="91"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="90"/>
+      <c r="B14" s="81"/>
+      <c r="C14" s="91"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="90"/>
+      <c r="B15" s="81"/>
+      <c r="C15" s="91"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="90"/>
+      <c r="B16" s="81"/>
+      <c r="C16" s="91"/>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="90"/>
+      <c r="B17" s="81"/>
+      <c r="C17" s="91"/>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="90"/>
+      <c r="B18" s="81"/>
+      <c r="C18" s="91"/>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="90"/>
+      <c r="B19" s="81"/>
+      <c r="C19" s="91"/>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="90"/>
+      <c r="B20" s="81"/>
+      <c r="C20" s="91"/>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="90"/>
+      <c r="B21" s="81"/>
+      <c r="C21" s="91"/>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="90"/>
+      <c r="B22" s="81"/>
+      <c r="C22" s="91"/>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="90"/>
+      <c r="B23" s="81"/>
+      <c r="C23" s="91"/>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="90"/>
+      <c r="B24" s="81"/>
+      <c r="C24" s="91"/>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="90"/>
+      <c r="B25" s="81"/>
+      <c r="C25" s="91"/>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="90"/>
+      <c r="B26" s="81"/>
+      <c r="C26" s="91"/>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="90"/>
+      <c r="B27" s="81"/>
+      <c r="C27" s="91"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="90"/>
+      <c r="B28" s="81"/>
+      <c r="C28" s="92"/>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="90"/>
+      <c r="B29" s="81"/>
+      <c r="C29" s="92"/>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="90"/>
+      <c r="B30" s="81"/>
+      <c r="C30" s="92"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="90"/>
+      <c r="B31" s="81"/>
+      <c r="C31" s="92"/>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="90"/>
+      <c r="B32" s="81"/>
+      <c r="C32" s="92"/>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="90"/>
+      <c r="B33" s="81"/>
+      <c r="C33" s="92"/>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="90"/>
+      <c r="B34" s="81"/>
+      <c r="C34" s="92"/>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="90"/>
+      <c r="B35" s="81"/>
+      <c r="C35" s="92"/>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="90"/>
+      <c r="B36" s="81"/>
+      <c r="C36" s="92"/>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="90"/>
+      <c r="B37" s="81"/>
+      <c r="C37" s="92"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="90"/>
+      <c r="B38" s="81"/>
+      <c r="C38" s="100"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="90"/>
+      <c r="B39" s="81"/>
+      <c r="C39" s="100"/>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="90"/>
+      <c r="B40" s="81"/>
+      <c r="C40" s="100"/>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="90"/>
+      <c r="B41" s="81"/>
+      <c r="C41" s="100"/>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="90"/>
+      <c r="B42" s="81"/>
+      <c r="C42" s="100"/>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="90"/>
+      <c r="B43" s="81"/>
+      <c r="C43" s="100"/>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="90"/>
+      <c r="B44" s="81"/>
+      <c r="C44" s="100"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="90"/>
+      <c r="B45" s="81"/>
+      <c r="C45" s="100"/>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="90"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="100"/>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="90"/>
+      <c r="B47" s="81"/>
+      <c r="C47" s="100"/>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="90"/>
+      <c r="B48" s="81"/>
+      <c r="C48" s="100"/>
     </row>
     <row r="49" spans="1:3">
-      <c r="B49" s="39"/>
+      <c r="A49" s="90"/>
+      <c r="B49" s="81"/>
+      <c r="C49" s="100"/>
     </row>
     <row r="50" spans="1:3">
-      <c r="B50" s="39"/>
+      <c r="A50" s="90"/>
+      <c r="B50" s="81"/>
+      <c r="C50" s="100"/>
     </row>
     <row r="51" spans="1:3">
-      <c r="B51" s="39"/>
+      <c r="A51" s="90"/>
+      <c r="B51" s="81"/>
+      <c r="C51" s="100"/>
     </row>
     <row r="52" spans="1:3">
-      <c r="B52" s="39"/>
+      <c r="A52" s="90"/>
+      <c r="B52" s="81"/>
+      <c r="C52" s="100"/>
     </row>
     <row r="53" spans="1:3">
-      <c r="B53" s="39"/>
+      <c r="A53" s="93"/>
+      <c r="B53" s="94"/>
+      <c r="C53" s="95"/>
     </row>
     <row r="54" spans="1:3">
+      <c r="A54" s="52"/>
       <c r="B54" s="35"/>
+      <c r="C54" s="55"/>
     </row>
     <row r="55" spans="1:3">
-      <c r="A55" s="46" t="s">
+      <c r="A55" s="87" t="s">
         <v>90</v>
       </c>
-      <c r="B55" s="39" t="s">
+      <c r="B55" s="88" t="s">
         <v>110</v>
       </c>
-      <c r="C55" s="39" t="s">
+      <c r="C55" s="89" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="56" spans="1:3">
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
+      <c r="A56" s="90"/>
+      <c r="B56" s="81"/>
+      <c r="C56" s="91"/>
     </row>
     <row r="57" spans="1:3">
-      <c r="B57" s="39"/>
-      <c r="C57" s="39"/>
+      <c r="A57" s="90"/>
+      <c r="B57" s="81"/>
+      <c r="C57" s="91"/>
     </row>
     <row r="58" spans="1:3">
-      <c r="B58" s="39"/>
-      <c r="C58" s="39"/>
+      <c r="A58" s="90"/>
+      <c r="B58" s="81"/>
+      <c r="C58" s="91"/>
     </row>
     <row r="59" spans="1:3">
-      <c r="B59" s="39"/>
-      <c r="C59" s="39"/>
+      <c r="A59" s="90"/>
+      <c r="B59" s="81"/>
+      <c r="C59" s="91"/>
     </row>
     <row r="60" spans="1:3">
-      <c r="B60" s="39"/>
-      <c r="C60" s="39"/>
+      <c r="A60" s="90"/>
+      <c r="B60" s="81"/>
+      <c r="C60" s="91"/>
     </row>
     <row r="61" spans="1:3">
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
+      <c r="A61" s="90"/>
+      <c r="B61" s="81"/>
+      <c r="C61" s="91"/>
     </row>
     <row r="62" spans="1:3">
-      <c r="B62" s="39"/>
-      <c r="C62" s="39"/>
+      <c r="A62" s="90"/>
+      <c r="B62" s="81"/>
+      <c r="C62" s="91"/>
     </row>
     <row r="63" spans="1:3">
-      <c r="B63" s="39"/>
-      <c r="C63" s="39"/>
+      <c r="A63" s="90"/>
+      <c r="B63" s="81"/>
+      <c r="C63" s="91"/>
     </row>
     <row r="64" spans="1:3">
-      <c r="B64" s="39"/>
-      <c r="C64" s="39"/>
-    </row>
-    <row r="65" spans="2:3">
-      <c r="B65" s="39"/>
-      <c r="C65" s="39"/>
-    </row>
-    <row r="66" spans="2:3">
-      <c r="B66" s="39"/>
-      <c r="C66" s="39"/>
-    </row>
-    <row r="67" spans="2:3">
-      <c r="B67" s="39"/>
-      <c r="C67" s="39"/>
-    </row>
-    <row r="68" spans="2:3">
-      <c r="B68" s="39"/>
-      <c r="C68" s="39"/>
-    </row>
-    <row r="69" spans="2:3">
-      <c r="B69" s="39"/>
-      <c r="C69" s="39"/>
-    </row>
-    <row r="70" spans="2:3">
-      <c r="B70" s="39"/>
-      <c r="C70" s="39"/>
-    </row>
-    <row r="71" spans="2:3">
-      <c r="B71" s="39"/>
-      <c r="C71" s="39"/>
-    </row>
-    <row r="72" spans="2:3">
-      <c r="B72" s="39"/>
-      <c r="C72" s="39"/>
-    </row>
-    <row r="73" spans="2:3">
-      <c r="B73" s="39"/>
-      <c r="C73" s="35"/>
-    </row>
-    <row r="74" spans="2:3">
-      <c r="B74" s="39"/>
-      <c r="C74" s="35"/>
-    </row>
-    <row r="75" spans="2:3">
-      <c r="B75" s="39"/>
-      <c r="C75" s="35"/>
-    </row>
-    <row r="76" spans="2:3">
-      <c r="B76" s="39"/>
-      <c r="C76" s="35"/>
-    </row>
-    <row r="77" spans="2:3">
-      <c r="B77" s="39"/>
-      <c r="C77" s="35"/>
-    </row>
-    <row r="78" spans="2:3">
-      <c r="B78" s="39"/>
-      <c r="C78" s="35"/>
-    </row>
-    <row r="79" spans="2:3">
-      <c r="B79" s="39"/>
-      <c r="C79" s="35"/>
-    </row>
-    <row r="80" spans="2:3">
-      <c r="B80" s="39"/>
-      <c r="C80" s="35"/>
-    </row>
-    <row r="81" spans="2:3">
-      <c r="B81" s="39"/>
-      <c r="C81" s="35"/>
-    </row>
-    <row r="82" spans="2:3">
-      <c r="B82" s="39"/>
-      <c r="C82" s="35"/>
-    </row>
-    <row r="83" spans="2:3">
-      <c r="B83" s="39"/>
-      <c r="C83" s="35"/>
-    </row>
-    <row r="84" spans="2:3">
-      <c r="B84" s="39"/>
-      <c r="C84" s="35"/>
-    </row>
-    <row r="85" spans="2:3">
-      <c r="B85" s="39"/>
-      <c r="C85" s="35"/>
-    </row>
-    <row r="86" spans="2:3">
-      <c r="B86" s="39"/>
-      <c r="C86" s="35"/>
-    </row>
-    <row r="87" spans="2:3">
-      <c r="B87" s="39"/>
-      <c r="C87" s="35"/>
-    </row>
-    <row r="88" spans="2:3">
-      <c r="B88" s="39"/>
-      <c r="C88" s="35"/>
-    </row>
-    <row r="89" spans="2:3">
-      <c r="B89" s="39"/>
-      <c r="C89" s="35"/>
-    </row>
-    <row r="90" spans="2:3">
-      <c r="B90" s="39"/>
-      <c r="C90" s="35"/>
-    </row>
-    <row r="91" spans="2:3">
-      <c r="B91" s="39"/>
-      <c r="C91" s="35"/>
-    </row>
-    <row r="92" spans="2:3">
-      <c r="B92" s="39"/>
-      <c r="C92" s="35"/>
-    </row>
-    <row r="93" spans="2:3">
-      <c r="B93" s="39"/>
-      <c r="C93" s="35"/>
-    </row>
-    <row r="94" spans="2:3">
-      <c r="B94" s="39"/>
-      <c r="C94" s="35"/>
-    </row>
-    <row r="95" spans="2:3">
-      <c r="B95" s="39"/>
-      <c r="C95" s="35"/>
-    </row>
-    <row r="96" spans="2:3">
-      <c r="B96" s="39"/>
+      <c r="A64" s="90"/>
+      <c r="B64" s="81"/>
+      <c r="C64" s="91"/>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" s="90"/>
+      <c r="B65" s="81"/>
+      <c r="C65" s="91"/>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" s="90"/>
+      <c r="B66" s="81"/>
+      <c r="C66" s="91"/>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" s="90"/>
+      <c r="B67" s="81"/>
+      <c r="C67" s="91"/>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" s="90"/>
+      <c r="B68" s="81"/>
+      <c r="C68" s="91"/>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" s="90"/>
+      <c r="B69" s="81"/>
+      <c r="C69" s="91"/>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" s="90"/>
+      <c r="B70" s="81"/>
+      <c r="C70" s="91"/>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" s="90"/>
+      <c r="B71" s="81"/>
+      <c r="C71" s="91"/>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" s="90"/>
+      <c r="B72" s="81"/>
+      <c r="C72" s="91"/>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" s="90"/>
+      <c r="B73" s="81"/>
+      <c r="C73" s="92"/>
+    </row>
+    <row r="74" spans="1:3">
+      <c r="A74" s="90"/>
+      <c r="B74" s="81"/>
+      <c r="C74" s="92"/>
+    </row>
+    <row r="75" spans="1:3">
+      <c r="A75" s="90"/>
+      <c r="B75" s="81"/>
+      <c r="C75" s="92"/>
+    </row>
+    <row r="76" spans="1:3">
+      <c r="A76" s="90"/>
+      <c r="B76" s="81"/>
+      <c r="C76" s="92"/>
+    </row>
+    <row r="77" spans="1:3">
+      <c r="A77" s="90"/>
+      <c r="B77" s="81"/>
+      <c r="C77" s="92"/>
+    </row>
+    <row r="78" spans="1:3">
+      <c r="A78" s="90"/>
+      <c r="B78" s="81"/>
+      <c r="C78" s="92"/>
+    </row>
+    <row r="79" spans="1:3">
+      <c r="A79" s="90"/>
+      <c r="B79" s="81"/>
+      <c r="C79" s="92"/>
+    </row>
+    <row r="80" spans="1:3">
+      <c r="A80" s="90"/>
+      <c r="B80" s="81"/>
+      <c r="C80" s="92"/>
+    </row>
+    <row r="81" spans="1:3">
+      <c r="A81" s="90"/>
+      <c r="B81" s="81"/>
+      <c r="C81" s="92"/>
+    </row>
+    <row r="82" spans="1:3">
+      <c r="A82" s="90"/>
+      <c r="B82" s="81"/>
+      <c r="C82" s="92"/>
+    </row>
+    <row r="83" spans="1:3">
+      <c r="A83" s="90"/>
+      <c r="B83" s="81"/>
+      <c r="C83" s="92"/>
+    </row>
+    <row r="84" spans="1:3">
+      <c r="A84" s="90"/>
+      <c r="B84" s="81"/>
+      <c r="C84" s="92"/>
+    </row>
+    <row r="85" spans="1:3">
+      <c r="A85" s="90"/>
+      <c r="B85" s="81"/>
+      <c r="C85" s="92"/>
+    </row>
+    <row r="86" spans="1:3">
+      <c r="A86" s="90"/>
+      <c r="B86" s="81"/>
+      <c r="C86" s="92"/>
+    </row>
+    <row r="87" spans="1:3">
+      <c r="A87" s="90"/>
+      <c r="B87" s="81"/>
+      <c r="C87" s="92"/>
+    </row>
+    <row r="88" spans="1:3">
+      <c r="A88" s="90"/>
+      <c r="B88" s="81"/>
+      <c r="C88" s="92"/>
+    </row>
+    <row r="89" spans="1:3">
+      <c r="A89" s="90"/>
+      <c r="B89" s="81"/>
+      <c r="C89" s="92"/>
+    </row>
+    <row r="90" spans="1:3">
+      <c r="A90" s="90"/>
+      <c r="B90" s="81"/>
+      <c r="C90" s="92"/>
+    </row>
+    <row r="91" spans="1:3">
+      <c r="A91" s="90"/>
+      <c r="B91" s="81"/>
+      <c r="C91" s="92"/>
+    </row>
+    <row r="92" spans="1:3">
+      <c r="A92" s="90"/>
+      <c r="B92" s="81"/>
+      <c r="C92" s="92"/>
+    </row>
+    <row r="93" spans="1:3">
+      <c r="A93" s="90"/>
+      <c r="B93" s="81"/>
+      <c r="C93" s="92"/>
+    </row>
+    <row r="94" spans="1:3">
+      <c r="A94" s="90"/>
+      <c r="B94" s="81"/>
+      <c r="C94" s="92"/>
+    </row>
+    <row r="95" spans="1:3">
+      <c r="A95" s="90"/>
+      <c r="B95" s="81"/>
+      <c r="C95" s="92"/>
+    </row>
+    <row r="96" spans="1:3">
+      <c r="A96" s="90"/>
+      <c r="B96" s="81"/>
+      <c r="C96" s="100"/>
     </row>
     <row r="97" spans="1:3">
-      <c r="B97" s="39"/>
+      <c r="A97" s="90"/>
+      <c r="B97" s="81"/>
+      <c r="C97" s="100"/>
     </row>
     <row r="98" spans="1:3">
-      <c r="B98" s="39"/>
+      <c r="A98" s="90"/>
+      <c r="B98" s="81"/>
+      <c r="C98" s="100"/>
     </row>
     <row r="99" spans="1:3">
-      <c r="B99" s="39"/>
+      <c r="A99" s="90"/>
+      <c r="B99" s="81"/>
+      <c r="C99" s="100"/>
     </row>
     <row r="100" spans="1:3">
-      <c r="B100" s="39"/>
+      <c r="A100" s="90"/>
+      <c r="B100" s="81"/>
+      <c r="C100" s="100"/>
     </row>
     <row r="101" spans="1:3">
-      <c r="B101" s="39"/>
+      <c r="A101" s="90"/>
+      <c r="B101" s="81"/>
+      <c r="C101" s="100"/>
     </row>
     <row r="102" spans="1:3">
-      <c r="B102" s="39"/>
+      <c r="A102" s="90"/>
+      <c r="B102" s="81"/>
+      <c r="C102" s="100"/>
     </row>
     <row r="103" spans="1:3">
-      <c r="B103" s="39"/>
-    </row>
-    <row r="104" spans="1:3">
-      <c r="B104" s="40"/>
+      <c r="A103" s="90"/>
+      <c r="B103" s="81"/>
+      <c r="C103" s="100"/>
+    </row>
+    <row r="104" spans="1:3" ht="17.250000">
+      <c r="A104" s="93"/>
+      <c r="B104" s="101"/>
+      <c r="C104" s="95"/>
+    </row>
+    <row r="105" spans="1:3">
+      <c r="A105" s="52"/>
+      <c r="B105" s="57"/>
+      <c r="C105" s="55"/>
     </row>
     <row r="106" spans="1:3">
-      <c r="A106" s="46" t="s">
+      <c r="A106" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="B106" s="39" t="s">
+      <c r="B106" s="88" t="s">
         <v>107</v>
       </c>
-      <c r="C106" s="39" t="s">
+      <c r="C106" s="89" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:3">
-      <c r="B107" s="39"/>
-      <c r="C107" s="39"/>
+      <c r="A107" s="90"/>
+      <c r="B107" s="81"/>
+      <c r="C107" s="91"/>
     </row>
     <row r="108" spans="1:3">
-      <c r="B108" s="39"/>
-      <c r="C108" s="39"/>
+      <c r="A108" s="90"/>
+      <c r="B108" s="81"/>
+      <c r="C108" s="91"/>
     </row>
     <row r="109" spans="1:3">
-      <c r="B109" s="39"/>
-      <c r="C109" s="39"/>
+      <c r="A109" s="90"/>
+      <c r="B109" s="81"/>
+      <c r="C109" s="91"/>
     </row>
     <row r="110" spans="1:3">
-      <c r="B110" s="39"/>
-      <c r="C110" s="39"/>
+      <c r="A110" s="90"/>
+      <c r="B110" s="81"/>
+      <c r="C110" s="91"/>
     </row>
     <row r="111" spans="1:3">
-      <c r="B111" s="39"/>
-      <c r="C111" s="39"/>
+      <c r="A111" s="90"/>
+      <c r="B111" s="81"/>
+      <c r="C111" s="91"/>
     </row>
     <row r="112" spans="1:3">
-      <c r="B112" s="39"/>
-      <c r="C112" s="39"/>
-    </row>
-    <row r="113" spans="2:3">
-      <c r="B113" s="39"/>
-      <c r="C113" s="39"/>
-    </row>
-    <row r="114" spans="2:3">
-      <c r="B114" s="39"/>
-      <c r="C114" s="39"/>
-    </row>
-    <row r="115" spans="2:3">
-      <c r="B115" s="39"/>
-      <c r="C115" s="39"/>
-    </row>
-    <row r="116" spans="2:3">
-      <c r="B116" s="39"/>
-      <c r="C116" s="39"/>
-    </row>
-    <row r="117" spans="2:3">
-      <c r="B117" s="39"/>
-      <c r="C117" s="39"/>
-    </row>
-    <row r="118" spans="2:3">
-      <c r="B118" s="39"/>
-      <c r="C118" s="39"/>
-    </row>
-    <row r="119" spans="2:3">
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-    </row>
-    <row r="120" spans="2:3">
-      <c r="B120" s="39"/>
-      <c r="C120" s="39"/>
-    </row>
-    <row r="121" spans="2:3">
-      <c r="B121" s="39"/>
-      <c r="C121" s="39"/>
-    </row>
-    <row r="122" spans="2:3">
-      <c r="B122" s="39"/>
-      <c r="C122" s="39"/>
-    </row>
-    <row r="123" spans="2:3">
-      <c r="B123" s="39"/>
-      <c r="C123" s="39"/>
-    </row>
-    <row r="124" spans="2:3">
-      <c r="B124" s="39"/>
-      <c r="C124" s="39"/>
-    </row>
-    <row r="125" spans="2:3">
-      <c r="B125" s="39"/>
-      <c r="C125" s="39"/>
-    </row>
-    <row r="126" spans="2:3">
-      <c r="B126" s="39"/>
-      <c r="C126" s="35"/>
-    </row>
-    <row r="127" spans="2:3">
-      <c r="B127" s="39"/>
-      <c r="C127" s="35"/>
-    </row>
-    <row r="128" spans="2:3">
-      <c r="B128" s="39"/>
-      <c r="C128" s="35"/>
+      <c r="A112" s="90"/>
+      <c r="B112" s="81"/>
+      <c r="C112" s="91"/>
+    </row>
+    <row r="113" spans="1:3">
+      <c r="A113" s="90"/>
+      <c r="B113" s="81"/>
+      <c r="C113" s="91"/>
+    </row>
+    <row r="114" spans="1:3">
+      <c r="A114" s="90"/>
+      <c r="B114" s="81"/>
+      <c r="C114" s="91"/>
+    </row>
+    <row r="115" spans="1:3">
+      <c r="A115" s="90"/>
+      <c r="B115" s="81"/>
+      <c r="C115" s="91"/>
+    </row>
+    <row r="116" spans="1:3">
+      <c r="A116" s="90"/>
+      <c r="B116" s="81"/>
+      <c r="C116" s="91"/>
+    </row>
+    <row r="117" spans="1:3">
+      <c r="A117" s="90"/>
+      <c r="B117" s="81"/>
+      <c r="C117" s="91"/>
+    </row>
+    <row r="118" spans="1:3">
+      <c r="A118" s="90"/>
+      <c r="B118" s="81"/>
+      <c r="C118" s="91"/>
+    </row>
+    <row r="119" spans="1:3">
+      <c r="A119" s="90"/>
+      <c r="B119" s="81"/>
+      <c r="C119" s="91"/>
+    </row>
+    <row r="120" spans="1:3">
+      <c r="A120" s="90"/>
+      <c r="B120" s="81"/>
+      <c r="C120" s="91"/>
+    </row>
+    <row r="121" spans="1:3">
+      <c r="A121" s="90"/>
+      <c r="B121" s="81"/>
+      <c r="C121" s="91"/>
+    </row>
+    <row r="122" spans="1:3">
+      <c r="A122" s="90"/>
+      <c r="B122" s="81"/>
+      <c r="C122" s="91"/>
+    </row>
+    <row r="123" spans="1:3">
+      <c r="A123" s="90"/>
+      <c r="B123" s="81"/>
+      <c r="C123" s="91"/>
+    </row>
+    <row r="124" spans="1:3">
+      <c r="A124" s="90"/>
+      <c r="B124" s="81"/>
+      <c r="C124" s="91"/>
+    </row>
+    <row r="125" spans="1:3">
+      <c r="A125" s="90"/>
+      <c r="B125" s="81"/>
+      <c r="C125" s="91"/>
+    </row>
+    <row r="126" spans="1:3">
+      <c r="A126" s="90"/>
+      <c r="B126" s="81"/>
+      <c r="C126" s="92"/>
+    </row>
+    <row r="127" spans="1:3">
+      <c r="A127" s="90"/>
+      <c r="B127" s="81"/>
+      <c r="C127" s="92"/>
+    </row>
+    <row r="128" spans="1:3">
+      <c r="A128" s="90"/>
+      <c r="B128" s="81"/>
+      <c r="C128" s="92"/>
     </row>
     <row r="129" spans="1:3">
-      <c r="B129" s="39"/>
-      <c r="C129" s="35"/>
+      <c r="A129" s="90"/>
+      <c r="B129" s="81"/>
+      <c r="C129" s="92"/>
     </row>
     <row r="130" spans="1:3">
-      <c r="B130" s="39"/>
-      <c r="C130" s="35"/>
-    </row>
-    <row r="131" spans="1:3">
-      <c r="B131" s="39"/>
-      <c r="C131" s="35"/>
+      <c r="A130" s="90"/>
+      <c r="B130" s="81"/>
+      <c r="C130" s="92"/>
+    </row>
+    <row r="131" spans="1:3" ht="17.250000">
+      <c r="A131" s="93"/>
+      <c r="B131" s="94"/>
+      <c r="C131" s="98"/>
     </row>
     <row r="132" spans="1:3">
-      <c r="C132" s="35"/>
+      <c r="A132" s="52"/>
+      <c r="B132" s="57"/>
+      <c r="C132" s="54"/>
     </row>
     <row r="133" spans="1:3">
-      <c r="A133" s="50" t="s">
+      <c r="A133" s="87" t="s">
         <v>116</v>
       </c>
-      <c r="B133" s="49" t="s">
+      <c r="B133" s="88" t="s">
         <v>145</v>
       </c>
-      <c r="C133" s="39" t="s">
+      <c r="C133" s="89" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="134" spans="1:3">
-      <c r="B134" s="39"/>
-      <c r="C134" s="39"/>
+      <c r="A134" s="90"/>
+      <c r="B134" s="81"/>
+      <c r="C134" s="91"/>
     </row>
     <row r="135" spans="1:3">
-      <c r="B135" s="39"/>
-      <c r="C135" s="39"/>
+      <c r="A135" s="90"/>
+      <c r="B135" s="81"/>
+      <c r="C135" s="91"/>
     </row>
     <row r="136" spans="1:3">
-      <c r="B136" s="39"/>
-      <c r="C136" s="39"/>
+      <c r="A136" s="90"/>
+      <c r="B136" s="81"/>
+      <c r="C136" s="91"/>
     </row>
     <row r="137" spans="1:3">
-      <c r="B137" s="39"/>
-      <c r="C137" s="39"/>
+      <c r="A137" s="90"/>
+      <c r="B137" s="81"/>
+      <c r="C137" s="91"/>
     </row>
     <row r="138" spans="1:3">
-      <c r="B138" s="39"/>
-      <c r="C138" s="39"/>
+      <c r="A138" s="90"/>
+      <c r="B138" s="81"/>
+      <c r="C138" s="91"/>
     </row>
     <row r="139" spans="1:3">
-      <c r="B139" s="39"/>
-      <c r="C139" s="39"/>
+      <c r="A139" s="90"/>
+      <c r="B139" s="81"/>
+      <c r="C139" s="91"/>
     </row>
     <row r="140" spans="1:3">
-      <c r="B140" s="39"/>
-      <c r="C140" s="39"/>
+      <c r="A140" s="90"/>
+      <c r="B140" s="81"/>
+      <c r="C140" s="91"/>
     </row>
     <row r="141" spans="1:3">
-      <c r="B141" s="39"/>
-      <c r="C141" s="39"/>
+      <c r="A141" s="90"/>
+      <c r="B141" s="81"/>
+      <c r="C141" s="91"/>
     </row>
     <row r="142" spans="1:3">
-      <c r="B142" s="39"/>
-      <c r="C142" s="35"/>
+      <c r="A142" s="90"/>
+      <c r="B142" s="81"/>
+      <c r="C142" s="92"/>
     </row>
     <row r="143" spans="1:3">
-      <c r="B143" s="39"/>
-      <c r="C143" s="35"/>
+      <c r="A143" s="90"/>
+      <c r="B143" s="81"/>
+      <c r="C143" s="92"/>
     </row>
     <row r="144" spans="1:3">
-      <c r="B144" s="39"/>
-      <c r="C144" s="35"/>
-    </row>
-    <row r="145" spans="2:3">
-      <c r="B145" s="39"/>
-      <c r="C145" s="35"/>
-    </row>
-    <row r="146" spans="2:3">
-      <c r="B146" s="39"/>
-      <c r="C146" s="35"/>
-    </row>
-    <row r="147" spans="2:3">
-      <c r="B147" s="39"/>
-      <c r="C147" s="35"/>
-    </row>
-    <row r="148" spans="2:3">
-      <c r="B148" s="39"/>
-    </row>
-    <row r="149" spans="2:3">
+      <c r="A144" s="90"/>
+      <c r="B144" s="81"/>
+      <c r="C144" s="92"/>
+    </row>
+    <row r="145" spans="1:3">
+      <c r="A145" s="90"/>
+      <c r="B145" s="81"/>
+      <c r="C145" s="92"/>
+    </row>
+    <row r="146" spans="1:3">
+      <c r="A146" s="90"/>
+      <c r="B146" s="81"/>
+      <c r="C146" s="92"/>
+    </row>
+    <row r="147" spans="1:3">
+      <c r="A147" s="90"/>
+      <c r="B147" s="81"/>
+      <c r="C147" s="92"/>
+    </row>
+    <row r="148" spans="1:3" ht="18.750000">
+      <c r="A148" s="93"/>
+      <c r="B148" s="94"/>
+      <c r="C148" s="95"/>
+    </row>
+    <row r="149" spans="1:3">
       <c r="B149" s="35"/>
     </row>
-    <row r="150" spans="2:3">
+    <row r="150" spans="1:3">
       <c r="B150" s="35"/>
     </row>
   </sheetData>

</xml_diff>